<commit_message>
clean up more columns of output
</commit_message>
<xml_diff>
--- a/mounts.xlsx
+++ b/mounts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="172">
   <si>
     <t>name</t>
   </si>
@@ -88,36 +88,24 @@
     <t>Axe Beak</t>
   </si>
   <si>
-    <t>1/4</t>
-  </si>
-  <si>
-    <t>3d10</t>
+    <t>3d10+1</t>
   </si>
   <si>
     <t>50 ft.</t>
   </si>
   <si>
-    <t>passive Perception 10</t>
-  </si>
-  <si>
     <t>Beak: Melee Weapon Attack: +4 to hit, reach 5 ft., one target. Hit: 6 (1d8 + 2) slashing damage.: 4: 1d8: 2</t>
   </si>
   <si>
     <t>Brown Bear</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>4d10</t>
+    <t>4d10+3</t>
   </si>
   <si>
     <t>40 ft., climb 30 ft.</t>
   </si>
   <si>
-    <t>passive Perception 13</t>
-  </si>
-  <si>
     <t>Keen Smell: The bear has advantage on Wisdom (Perception) checks that rely on smell.: 0</t>
   </si>
   <si>
@@ -133,13 +121,7 @@
     <t>Camel</t>
   </si>
   <si>
-    <t>1/8</t>
-  </si>
-  <si>
-    <t>2d10</t>
-  </si>
-  <si>
-    <t>passive Perception 9</t>
+    <t>2d10+2</t>
   </si>
   <si>
     <t>Bite: Melee Weapon Attack: +5 to hit, reach 5 ft., one target. Hit: 2 (1d4) bludgeoning damage.: 5: 1d4</t>
@@ -148,16 +130,13 @@
     <t>Cave Bear</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>5d10</t>
+    <t>5d10+3</t>
   </si>
   <si>
     <t>40 ft., swim 30 ft.</t>
   </si>
   <si>
-    <t>darkvision 60 ft., passive Perception 13</t>
+    <t>darkvision 60 ft.</t>
   </si>
   <si>
     <t>Bite: Melee Weapon Attack: +7 to hit, reach 5 ft., one target. Hit: 9 (1d8 + 5) piercing damage.: 7: 1d8: 5</t>
@@ -169,10 +148,13 @@
     <t>Constrictor Snake</t>
   </si>
   <si>
+    <t>2d10+1</t>
+  </si>
+  <si>
     <t>30 ft., swim 30 ft.</t>
   </si>
   <si>
-    <t>blindsight 10 ft., passive Perception 10</t>
+    <t>blindsight 10 ft.</t>
   </si>
   <si>
     <t>Bite: Melee Weapon Attack: +4 to hit, reach 5 ft., one creature. Hit: 5 (1d6 + 2) piercing damage.: 4: 1d6: 2</t>
@@ -184,9 +166,6 @@
     <t>Crocodile</t>
   </si>
   <si>
-    <t>1/2</t>
-  </si>
-  <si>
     <t>20 ft., swim 20 ft.</t>
   </si>
   <si>
@@ -199,6 +178,9 @@
     <t>Dire Wolf</t>
   </si>
   <si>
+    <t>5d10+2</t>
+  </si>
+  <si>
     <t>Keen Hearing and Smell: The wolf has advantage on Wisdom (Perception) checks that rely on hearing or smell.: 0</t>
   </si>
   <si>
@@ -232,10 +214,13 @@
     <t>Giant Bat</t>
   </si>
   <si>
+    <t>4d10+0</t>
+  </si>
+  <si>
     <t>10 ft., fly 60 ft.</t>
   </si>
   <si>
-    <t>blindsight 60 ft., passive Perception 11</t>
+    <t>blindsight 60 ft.</t>
   </si>
   <si>
     <t>Echolocation: The bat can't use its blindsight while deafened.: 0</t>
@@ -247,9 +232,6 @@
     <t>Giant Boar</t>
   </si>
   <si>
-    <t>passive Perception 8</t>
-  </si>
-  <si>
     <t>Charge: If the boar moves at least 20 ft. straight toward a target and then hits it with a tusk attack on the same turn, the target takes an extra 7 (2d6) slashing damage. If the target is a creature, it must succeed on a DC 13 Strength saving throw or be knocked prone.: 0: 2d6</t>
   </si>
   <si>
@@ -262,12 +244,12 @@
     <t>Giant Eagle</t>
   </si>
   <si>
+    <t>4d10+1</t>
+  </si>
+  <si>
     <t>10 ft., fly 80 ft.</t>
   </si>
   <si>
-    <t>passive Perception 14</t>
-  </si>
-  <si>
     <t>Keen Sight: The eagle has advantage on Wisdom (Perception) checks that rely on sight.: 0</t>
   </si>
   <si>
@@ -286,9 +268,6 @@
     <t>Giant Goat</t>
   </si>
   <si>
-    <t>passive Perception 11</t>
-  </si>
-  <si>
     <t>Charge: If the goat moves at least 20 ft. straight toward a target and then hits it with a ram attack on the same turn, the target takes an extra 5 (2d4) bludgeoning damage. If the target is a creature, it must succeed on a DC 13 Strength saving throw or be knocked prone.: 0: 2d4</t>
   </si>
   <si>
@@ -301,7 +280,7 @@
     <t>Giant Hyena</t>
   </si>
   <si>
-    <t>6d10</t>
+    <t>6d10+2</t>
   </si>
   <si>
     <t>Rampage: When the hyena reduces a creature to 0 hit points with a melee attack on its turn, the hyena can take a bonus action to move up to half its speed and make a bite attack.: 0</t>
@@ -316,7 +295,7 @@
     <t>30 ft., climb 30 ft.</t>
   </si>
   <si>
-    <t>darkvision 30 ft., passive Perception 10</t>
+    <t>darkvision 30 ft.</t>
   </si>
   <si>
     <t>Variant: Hold Breath: The lizard can hold its breath for 15 minutes. (A lizard that has this trait also has a swimming speed of 30 feet.): 0</t>
@@ -331,15 +310,12 @@
     <t>Giant Octopus</t>
   </si>
   <si>
-    <t>8d10</t>
+    <t>8d10+1</t>
   </si>
   <si>
     <t>10 ft., swim 60 ft.</t>
   </si>
   <si>
-    <t>darkvision 60 ft., passive Perception 14</t>
-  </si>
-  <si>
     <t>Hold Breath: While out of water, the octopus can hold its breath for 1 hour.: 0</t>
   </si>
   <si>
@@ -361,7 +337,7 @@
     <t>5 ft., fly 60 ft.</t>
   </si>
   <si>
-    <t>darkvision 120 ft., passive Perception 15</t>
+    <t>darkvision 120 ft.</t>
   </si>
   <si>
     <t>Flyby: The owl doesn't provoke opportunity attacks when it flies out of an enemy's reach.: 0</t>
@@ -379,13 +355,7 @@
     <t>Giant Scorpion</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>7d10</t>
-  </si>
-  <si>
-    <t>blindsight 60 ft., passive Perception 9</t>
+    <t>7d10+2</t>
   </si>
   <si>
     <t>Claw: Melee Weapon Attack: +4 to hit, reach 5 ft., one target. Hit: 6 (1d8 + 2) bludgeoning damage, and the target is grappled (escape DC 12). The scorpion has two claws, each of which can grapple only one target.: 4: 1d8: 2</t>
@@ -400,6 +370,9 @@
     <t>Giant Sea Horse</t>
   </si>
   <si>
+    <t>3d10+0</t>
+  </si>
+  <si>
     <t>0 ft., swim 40 ft.</t>
   </si>
   <si>
@@ -415,7 +388,7 @@
     <t>Giant Spider</t>
   </si>
   <si>
-    <t>blindsight 10 ft., darkvision 60 ft., passive Perception 10</t>
+    <t>blindsight 10 ft., darkvision 60 ft.</t>
   </si>
   <si>
     <t>Spider Climb: The spider can climb difficult surfaces, including upside down on ceilings, without needing to make an ability check.: 0</t>
@@ -434,6 +407,9 @@
   </si>
   <si>
     <t>Giant Toad</t>
+  </si>
+  <si>
+    <t>6d10+1</t>
   </si>
   <si>
     <t>20 ft., swim 40 ft.</t>
@@ -458,9 +434,6 @@
     <t>swim 40 ft.</t>
   </si>
   <si>
-    <t>darkvision 30 ft., passive Perception 12</t>
-  </si>
-  <si>
     <t>Blood Frenzy: The shark has advantage on melee attack rolls against any creature that doesn't have all its hit points.: 0</t>
   </si>
   <si>
@@ -492,6 +465,9 @@
   </si>
   <si>
     <t>Plesiosaurus</t>
+  </si>
+  <si>
+    <t>8d10+3</t>
   </si>
   <si>
     <t>Hold Breath: The plesiosaurus can hold its breath for 1 hour.: 0</t>
@@ -986,20 +962,20 @@
       <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
+      <c r="B2" t="n">
+        <v>0.25</v>
       </c>
       <c r="C2" t="n">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" t="n">
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" t="n">
         <v>14</v>
@@ -1019,9 +995,7 @@
       <c r="L2" t="n">
         <v>5</v>
       </c>
-      <c r="M2" t="s">
-        <v>27</v>
-      </c>
+      <c r="M2" t="s"/>
       <c r="N2" t="s"/>
       <c r="O2" t="s"/>
       <c r="P2" t="s"/>
@@ -1029,7 +1003,7 @@
       <c r="R2" t="s"/>
       <c r="S2" t="s"/>
       <c r="T2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="U2" t="s"/>
       <c r="V2" t="s"/>
@@ -1037,22 +1011,22 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
       </c>
       <c r="C3" t="n">
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E3" t="n">
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G3" t="n">
         <v>19</v>
@@ -1072,48 +1046,46 @@
       <c r="L3" t="n">
         <v>7</v>
       </c>
-      <c r="M3" t="s">
-        <v>33</v>
-      </c>
+      <c r="M3" t="s"/>
       <c r="N3" t="n">
         <v>3</v>
       </c>
       <c r="O3" t="s"/>
       <c r="P3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="Q3" t="s"/>
       <c r="R3" t="s"/>
       <c r="S3" t="s"/>
       <c r="T3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="U3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="W3" t="s"/>
     </row>
     <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.125</v>
       </c>
       <c r="C4" t="n">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E4" t="n">
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" t="n">
         <v>16</v>
@@ -1133,9 +1105,7 @@
       <c r="L4" t="n">
         <v>5</v>
       </c>
-      <c r="M4" t="s">
-        <v>41</v>
-      </c>
+      <c r="M4" t="s"/>
       <c r="N4" t="s"/>
       <c r="O4" t="s"/>
       <c r="P4" t="s"/>
@@ -1143,7 +1113,7 @@
       <c r="R4" t="s"/>
       <c r="S4" t="s"/>
       <c r="T4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="U4" t="s"/>
       <c r="V4" t="s"/>
@@ -1151,22 +1121,22 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" t="s">
-        <v>44</v>
+        <v>37</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
       </c>
       <c r="C5" t="n">
         <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E5" t="n">
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G5" t="n">
         <v>20</v>
@@ -1187,47 +1157,47 @@
         <v>7</v>
       </c>
       <c r="M5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="N5" t="n">
         <v>3</v>
       </c>
       <c r="O5" t="s"/>
       <c r="P5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="Q5" t="s"/>
       <c r="R5" t="s"/>
       <c r="S5" t="s"/>
       <c r="T5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="U5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="V5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="W5" t="s"/>
     </row>
     <row r="6" spans="1:23">
       <c r="A6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
+        <v>43</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.25</v>
       </c>
       <c r="C6" t="n">
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E6" t="n">
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G6" t="n">
         <v>15</v>
@@ -1248,7 +1218,7 @@
         <v>3</v>
       </c>
       <c r="M6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="N6" t="s"/>
       <c r="O6" t="s"/>
@@ -1257,32 +1227,32 @@
       <c r="R6" t="s"/>
       <c r="S6" t="s"/>
       <c r="T6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="U6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="V6" t="s"/>
       <c r="W6" t="s"/>
     </row>
     <row r="7" spans="1:23">
       <c r="A7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
+        <v>49</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.5</v>
       </c>
       <c r="C7" t="n">
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" t="n">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G7" t="n">
         <v>15</v>
@@ -1302,21 +1272,19 @@
       <c r="L7" t="n">
         <v>5</v>
       </c>
-      <c r="M7" t="s">
-        <v>27</v>
-      </c>
+      <c r="M7" t="s"/>
       <c r="N7" t="s"/>
       <c r="O7" t="n">
         <v>2</v>
       </c>
       <c r="P7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="Q7" t="s"/>
       <c r="R7" t="s"/>
       <c r="S7" t="s"/>
       <c r="T7" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="U7" t="s"/>
       <c r="V7" t="s"/>
@@ -1324,22 +1292,22 @@
     </row>
     <row r="8" spans="1:23">
       <c r="A8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
+        <v>53</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
       </c>
       <c r="C8" t="n">
         <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="E8" t="n">
         <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" t="n">
         <v>17</v>
@@ -1359,9 +1327,7 @@
       <c r="L8" t="n">
         <v>7</v>
       </c>
-      <c r="M8" t="s">
-        <v>33</v>
-      </c>
+      <c r="M8" t="s"/>
       <c r="N8" t="n">
         <v>3</v>
       </c>
@@ -1369,15 +1335,15 @@
         <v>4</v>
       </c>
       <c r="P8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="Q8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="R8" t="s"/>
       <c r="S8" t="s"/>
       <c r="T8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="U8" t="s"/>
       <c r="V8" t="s"/>
@@ -1385,22 +1351,22 @@
     </row>
     <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
+        <v>58</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.25</v>
       </c>
       <c r="C9" t="n">
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" t="n">
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G9" t="n">
         <v>18</v>
@@ -1420,9 +1386,7 @@
       <c r="L9" t="n">
         <v>7</v>
       </c>
-      <c r="M9" t="s">
-        <v>27</v>
-      </c>
+      <c r="M9" t="s"/>
       <c r="N9" t="s"/>
       <c r="O9" t="s"/>
       <c r="P9" t="s"/>
@@ -1430,7 +1394,7 @@
       <c r="R9" t="s"/>
       <c r="S9" t="s"/>
       <c r="T9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="U9" t="s"/>
       <c r="V9" t="s"/>
@@ -1438,22 +1402,22 @@
     </row>
     <row r="10" spans="1:23">
       <c r="A10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
+        <v>61</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.25</v>
       </c>
       <c r="C10" t="n">
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E10" t="n">
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" t="n">
         <v>16</v>
@@ -1473,44 +1437,42 @@
       <c r="L10" t="n">
         <v>6</v>
       </c>
-      <c r="M10" t="s">
-        <v>27</v>
-      </c>
+      <c r="M10" t="s"/>
       <c r="N10" t="s"/>
       <c r="O10" t="s"/>
       <c r="P10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="Q10" t="s"/>
       <c r="R10" t="s"/>
       <c r="S10" t="s"/>
       <c r="T10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="U10" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="V10" t="s"/>
       <c r="W10" t="s"/>
     </row>
     <row r="11" spans="1:23">
       <c r="A11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
+        <v>65</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.25</v>
       </c>
       <c r="C11" t="n">
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="E11" t="n">
         <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G11" t="n">
         <v>15</v>
@@ -1531,20 +1493,20 @@
         <v>6</v>
       </c>
       <c r="M11" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="N11" t="s"/>
       <c r="O11" t="s"/>
       <c r="P11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="Q11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="R11" t="s"/>
       <c r="S11" t="s"/>
       <c r="T11" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="U11" t="s"/>
       <c r="V11" t="s"/>
@@ -1552,22 +1514,22 @@
     </row>
     <row r="12" spans="1:23">
       <c r="A12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" t="s">
-        <v>44</v>
+        <v>71</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2</v>
       </c>
       <c r="C12" t="n">
         <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E12" t="n">
         <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G12" t="n">
         <v>17</v>
@@ -1587,21 +1549,19 @@
       <c r="L12" t="n">
         <v>5</v>
       </c>
-      <c r="M12" t="s">
-        <v>77</v>
-      </c>
+      <c r="M12" t="s"/>
       <c r="N12" t="s"/>
       <c r="O12" t="s"/>
       <c r="P12" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="Q12" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="R12" t="s"/>
       <c r="S12" t="s"/>
       <c r="T12" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="U12" t="s"/>
       <c r="V12" t="s"/>
@@ -1609,22 +1569,22 @@
     </row>
     <row r="13" spans="1:23">
       <c r="A13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
+        <v>75</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
       </c>
       <c r="C13" t="n">
         <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="E13" t="n">
         <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G13" t="n">
         <v>16</v>
@@ -1644,50 +1604,48 @@
       <c r="L13" t="n">
         <v>10</v>
       </c>
-      <c r="M13" t="s">
-        <v>83</v>
-      </c>
+      <c r="M13" t="s"/>
       <c r="N13" t="n">
         <v>4</v>
       </c>
       <c r="O13" t="s"/>
       <c r="P13" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="Q13" t="s"/>
       <c r="R13" t="s"/>
       <c r="S13" t="s"/>
       <c r="T13" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="U13" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="V13" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="W13" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:23">
       <c r="A14" t="s">
-        <v>89</v>
-      </c>
-      <c r="B14" t="s">
-        <v>56</v>
+        <v>83</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.5</v>
       </c>
       <c r="C14" t="n">
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" t="n">
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G14" t="n">
         <v>17</v>
@@ -1707,21 +1665,19 @@
       <c r="L14" t="n">
         <v>6</v>
       </c>
-      <c r="M14" t="s">
-        <v>90</v>
-      </c>
+      <c r="M14" t="s"/>
       <c r="N14" t="s"/>
       <c r="O14" t="s"/>
       <c r="P14" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="Q14" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="R14" t="s"/>
       <c r="S14" t="s"/>
       <c r="T14" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="U14" t="s"/>
       <c r="V14" t="s"/>
@@ -1729,22 +1685,22 @@
     </row>
     <row r="15" spans="1:23">
       <c r="A15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
+        <v>87</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
       </c>
       <c r="C15" t="n">
         <v>45</v>
       </c>
       <c r="D15" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E15" t="n">
         <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G15" t="n">
         <v>16</v>
@@ -1764,21 +1720,19 @@
       <c r="L15" t="n">
         <v>7</v>
       </c>
-      <c r="M15" t="s">
-        <v>33</v>
-      </c>
+      <c r="M15" t="s"/>
       <c r="N15" t="n">
         <v>3</v>
       </c>
       <c r="O15" t="s"/>
       <c r="P15" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="Q15" t="s"/>
       <c r="R15" t="s"/>
       <c r="S15" t="s"/>
       <c r="T15" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="U15" t="s"/>
       <c r="V15" t="s"/>
@@ -1786,22 +1740,22 @@
     </row>
     <row r="16" spans="1:23">
       <c r="A16" t="s">
-        <v>98</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
+        <v>91</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.25</v>
       </c>
       <c r="C16" t="n">
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" t="n">
         <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="G16" t="n">
         <v>15</v>
@@ -1822,20 +1776,20 @@
         <v>5</v>
       </c>
       <c r="M16" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="N16" t="s"/>
       <c r="O16" t="s"/>
       <c r="P16" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="Q16" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="R16" t="s"/>
       <c r="S16" t="s"/>
       <c r="T16" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="U16" t="s"/>
       <c r="V16" t="s"/>
@@ -1843,22 +1797,22 @@
     </row>
     <row r="17" spans="1:23">
       <c r="A17" t="s">
-        <v>104</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
+        <v>97</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
       </c>
       <c r="C17" t="n">
         <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E17" t="n">
         <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G17" t="n">
         <v>17</v>
@@ -1879,7 +1833,7 @@
         <v>4</v>
       </c>
       <c r="M17" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="N17" t="n">
         <v>4</v>
@@ -1888,42 +1842,42 @@
         <v>5</v>
       </c>
       <c r="P17" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="Q17" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="R17" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="S17" t="s"/>
       <c r="T17" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="U17" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="V17" t="s"/>
       <c r="W17" t="s"/>
     </row>
     <row r="18" spans="1:23">
       <c r="A18" t="s">
-        <v>113</v>
-      </c>
-      <c r="B18" t="s">
-        <v>24</v>
+        <v>105</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.25</v>
       </c>
       <c r="C18" t="n">
         <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18" t="n">
         <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="G18" t="n">
         <v>13</v>
@@ -1944,7 +1898,7 @@
         <v>10</v>
       </c>
       <c r="M18" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="N18" t="n">
         <v>5</v>
@@ -1953,40 +1907,40 @@
         <v>4</v>
       </c>
       <c r="P18" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="Q18" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="R18" t="s"/>
       <c r="S18" t="s"/>
       <c r="T18" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="U18" t="s"/>
       <c r="V18" t="s"/>
       <c r="W18" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:23">
       <c r="A19" t="s">
-        <v>120</v>
-      </c>
-      <c r="B19" t="s">
-        <v>121</v>
+        <v>112</v>
+      </c>
+      <c r="B19" t="n">
+        <v>3</v>
       </c>
       <c r="C19" t="n">
         <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="E19" t="n">
         <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G19" t="n">
         <v>15</v>
@@ -2007,7 +1961,7 @@
         <v>3</v>
       </c>
       <c r="M19" t="s">
-        <v>123</v>
+        <v>68</v>
       </c>
       <c r="N19" t="s"/>
       <c r="O19" t="s"/>
@@ -2016,34 +1970,34 @@
       <c r="R19" t="s"/>
       <c r="S19" t="s"/>
       <c r="T19" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="U19" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="V19" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="W19" t="s"/>
     </row>
     <row r="20" spans="1:23">
       <c r="A20" t="s">
-        <v>127</v>
-      </c>
-      <c r="B20" t="s">
-        <v>56</v>
+        <v>117</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.5</v>
       </c>
       <c r="C20" t="n">
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>118</v>
       </c>
       <c r="E20" t="n">
         <v>13</v>
       </c>
       <c r="F20" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="G20" t="n">
         <v>12</v>
@@ -2063,21 +2017,19 @@
       <c r="L20" t="n">
         <v>5</v>
       </c>
-      <c r="M20" t="s">
-        <v>90</v>
-      </c>
+      <c r="M20" t="s"/>
       <c r="N20" t="s"/>
       <c r="O20" t="s"/>
       <c r="P20" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="Q20" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="R20" t="s"/>
       <c r="S20" t="s"/>
       <c r="T20" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="U20" t="s"/>
       <c r="V20" t="s"/>
@@ -2085,22 +2037,22 @@
     </row>
     <row r="21" spans="1:23">
       <c r="A21" t="s">
-        <v>132</v>
-      </c>
-      <c r="B21" t="s">
-        <v>30</v>
+        <v>123</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
       </c>
       <c r="C21" t="n">
         <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="E21" t="n">
         <v>14</v>
       </c>
       <c r="F21" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="G21" t="n">
         <v>14</v>
@@ -2121,49 +2073,49 @@
         <v>4</v>
       </c>
       <c r="M21" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="N21" t="s"/>
       <c r="O21" t="n">
         <v>7</v>
       </c>
       <c r="P21" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="Q21" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="R21" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="S21" t="s"/>
       <c r="T21" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="U21" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="V21" t="s"/>
       <c r="W21" t="s"/>
     </row>
     <row r="22" spans="1:23">
       <c r="A22" t="s">
-        <v>139</v>
-      </c>
-      <c r="B22" t="s">
-        <v>30</v>
+        <v>130</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
       </c>
       <c r="C22" t="n">
         <v>39</v>
       </c>
       <c r="D22" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="E22" t="n">
         <v>11</v>
       </c>
       <c r="F22" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="G22" t="n">
         <v>15</v>
@@ -2184,45 +2136,45 @@
         <v>3</v>
       </c>
       <c r="M22" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="N22" t="s"/>
       <c r="O22" t="s"/>
       <c r="P22" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="Q22" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="R22" t="s"/>
       <c r="S22" t="s"/>
       <c r="T22" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="U22" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="V22" t="s"/>
       <c r="W22" t="s"/>
     </row>
     <row r="23" spans="1:23">
       <c r="A23" t="s">
-        <v>145</v>
-      </c>
-      <c r="B23" t="s">
-        <v>44</v>
+        <v>137</v>
+      </c>
+      <c r="B23" t="n">
+        <v>2</v>
       </c>
       <c r="C23" t="n">
         <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E23" t="n">
         <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="G23" t="n">
         <v>18</v>
@@ -2243,22 +2195,22 @@
         <v>4</v>
       </c>
       <c r="M23" t="s">
-        <v>147</v>
+        <v>93</v>
       </c>
       <c r="N23" t="n">
         <v>2</v>
       </c>
       <c r="O23" t="s"/>
       <c r="P23" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="Q23" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="R23" t="s"/>
       <c r="S23" t="s"/>
       <c r="T23" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="U23" t="s"/>
       <c r="V23" t="s"/>
@@ -2266,22 +2218,22 @@
     </row>
     <row r="24" spans="1:23">
       <c r="A24" t="s">
-        <v>151</v>
-      </c>
-      <c r="B24" t="s">
-        <v>30</v>
+        <v>142</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
       </c>
       <c r="C24" t="n">
         <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="E24" t="n">
         <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G24" t="n">
         <v>17</v>
@@ -2301,9 +2253,7 @@
       <c r="L24" t="n">
         <v>8</v>
       </c>
-      <c r="M24" t="s">
-        <v>33</v>
-      </c>
+      <c r="M24" t="s"/>
       <c r="N24" t="n">
         <v>3</v>
       </c>
@@ -2311,44 +2261,44 @@
         <v>6</v>
       </c>
       <c r="P24" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="Q24" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="R24" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="S24" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="T24" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="U24" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="V24" t="s"/>
       <c r="W24" t="s"/>
     </row>
     <row r="25" spans="1:23">
       <c r="A25" t="s">
-        <v>158</v>
-      </c>
-      <c r="B25" t="s">
-        <v>44</v>
+        <v>149</v>
+      </c>
+      <c r="B25" t="n">
+        <v>2</v>
       </c>
       <c r="C25" t="n">
         <v>68</v>
       </c>
       <c r="D25" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="E25" t="n">
         <v>13</v>
       </c>
       <c r="F25" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="G25" t="n">
         <v>18</v>
@@ -2368,9 +2318,7 @@
       <c r="L25" t="n">
         <v>5</v>
       </c>
-      <c r="M25" t="s">
-        <v>33</v>
-      </c>
+      <c r="M25" t="s"/>
       <c r="N25" t="n">
         <v>3</v>
       </c>
@@ -2378,13 +2326,13 @@
         <v>4</v>
       </c>
       <c r="P25" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="Q25" t="s"/>
       <c r="R25" t="s"/>
       <c r="S25" t="s"/>
       <c r="T25" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="U25" t="s"/>
       <c r="V25" t="s"/>
@@ -2392,22 +2340,22 @@
     </row>
     <row r="26" spans="1:23">
       <c r="A26" t="s">
-        <v>161</v>
-      </c>
-      <c r="B26" t="s">
-        <v>44</v>
+        <v>153</v>
+      </c>
+      <c r="B26" t="n">
+        <v>2</v>
       </c>
       <c r="C26" t="n">
         <v>42</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E26" t="n">
         <v>12</v>
       </c>
       <c r="F26" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G26" t="n">
         <v>20</v>
@@ -2427,48 +2375,46 @@
       <c r="L26" t="n">
         <v>7</v>
       </c>
-      <c r="M26" t="s">
-        <v>33</v>
-      </c>
+      <c r="M26" t="s"/>
       <c r="N26" t="n">
         <v>3</v>
       </c>
       <c r="O26" t="s"/>
       <c r="P26" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="Q26" t="s"/>
       <c r="R26" t="s"/>
       <c r="S26" t="s"/>
       <c r="T26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="U26" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="V26" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="W26" t="s"/>
     </row>
     <row r="27" spans="1:23">
       <c r="A27" t="s">
-        <v>162</v>
-      </c>
-      <c r="B27" t="s">
-        <v>44</v>
+        <v>154</v>
+      </c>
+      <c r="B27" t="n">
+        <v>2</v>
       </c>
       <c r="C27" t="n">
         <v>45</v>
       </c>
       <c r="D27" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E27" t="n">
         <v>11</v>
       </c>
       <c r="F27" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G27" t="n">
         <v>21</v>
@@ -2488,19 +2434,17 @@
       <c r="L27" t="n">
         <v>6</v>
       </c>
-      <c r="M27" t="s">
-        <v>90</v>
-      </c>
+      <c r="M27" t="s"/>
       <c r="N27" t="s"/>
       <c r="O27" t="s"/>
       <c r="P27" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="Q27" t="s"/>
       <c r="R27" t="s"/>
       <c r="S27" t="s"/>
       <c r="T27" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="U27" t="s"/>
       <c r="V27" t="s"/>
@@ -2508,22 +2452,22 @@
     </row>
     <row r="28" spans="1:23">
       <c r="A28" t="s">
-        <v>165</v>
-      </c>
-      <c r="B28" t="s">
-        <v>24</v>
+        <v>157</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0.25</v>
       </c>
       <c r="C28" t="n">
         <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E28" t="n">
         <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="G28" t="n">
         <v>16</v>
@@ -2543,9 +2487,7 @@
       <c r="L28" t="n">
         <v>7</v>
       </c>
-      <c r="M28" t="s">
-        <v>27</v>
-      </c>
+      <c r="M28" t="s"/>
       <c r="N28" t="s"/>
       <c r="O28" t="s"/>
       <c r="P28" t="s"/>
@@ -2553,7 +2495,7 @@
       <c r="R28" t="s"/>
       <c r="S28" t="s"/>
       <c r="T28" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="U28" t="s"/>
       <c r="V28" t="s"/>
@@ -2561,22 +2503,22 @@
     </row>
     <row r="29" spans="1:23">
       <c r="A29" t="s">
-        <v>168</v>
-      </c>
-      <c r="B29" t="s">
-        <v>44</v>
+        <v>160</v>
+      </c>
+      <c r="B29" t="n">
+        <v>2</v>
       </c>
       <c r="C29" t="n">
         <v>52</v>
       </c>
       <c r="D29" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="E29" t="n">
         <v>12</v>
       </c>
       <c r="F29" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G29" t="n">
         <v>18</v>
@@ -2596,9 +2538,7 @@
       <c r="L29" t="n">
         <v>8</v>
       </c>
-      <c r="M29" t="s">
-        <v>33</v>
-      </c>
+      <c r="M29" t="s"/>
       <c r="N29" t="n">
         <v>3</v>
       </c>
@@ -2606,40 +2546,40 @@
         <v>6</v>
       </c>
       <c r="P29" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="Q29" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="R29" t="s"/>
       <c r="S29" t="s"/>
       <c r="T29" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="U29" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="V29" t="s"/>
       <c r="W29" t="s"/>
     </row>
     <row r="30" spans="1:23">
       <c r="A30" t="s">
-        <v>173</v>
-      </c>
-      <c r="B30" t="s">
-        <v>30</v>
+        <v>165</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1</v>
       </c>
       <c r="C30" t="n">
         <v>37</v>
       </c>
       <c r="D30" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="E30" t="n">
         <v>12</v>
       </c>
       <c r="F30" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G30" t="n">
         <v>17</v>
@@ -2660,7 +2600,7 @@
         <v>8</v>
       </c>
       <c r="M30" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="N30" t="n">
         <v>3</v>
@@ -2669,40 +2609,40 @@
         <v>6</v>
       </c>
       <c r="P30" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="Q30" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="R30" t="s"/>
       <c r="S30" t="s"/>
       <c r="T30" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="U30" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="V30" t="s"/>
       <c r="W30" t="s"/>
     </row>
     <row r="31" spans="1:23">
       <c r="A31" t="s">
-        <v>177</v>
-      </c>
-      <c r="B31" t="s">
-        <v>56</v>
+        <v>169</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0.5</v>
       </c>
       <c r="C31" t="n">
         <v>19</v>
       </c>
       <c r="D31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E31" t="n">
         <v>11</v>
       </c>
       <c r="F31" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="G31" t="n">
         <v>18</v>
@@ -2722,19 +2662,17 @@
       <c r="L31" t="n">
         <v>7</v>
       </c>
-      <c r="M31" t="s">
-        <v>90</v>
-      </c>
+      <c r="M31" t="s"/>
       <c r="N31" t="s"/>
       <c r="O31" t="s"/>
       <c r="P31" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="Q31" t="s"/>
       <c r="R31" t="s"/>
       <c r="S31" t="s"/>
       <c r="T31" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="U31" t="s"/>
       <c r="V31" t="s"/>

</xml_diff>